<commit_message>
[ANV] added some Hang stuff to decay chains spreadsheet
</commit_message>
<xml_diff>
--- a/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
+++ b/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEA7164-FC05-EA49-ADFE-2DCDBE14B1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69141C50-D66F-6249-AD3A-72B8862BA34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
     <sheet name="U235" sheetId="2" r:id="rId2"/>
     <sheet name="U238" sheetId="3" r:id="rId3"/>
     <sheet name="SE Results" sheetId="4" r:id="rId4"/>
-    <sheet name="Shotcrete Density" sheetId="5" r:id="rId5"/>
-    <sheet name="1ppb" sheetId="6" r:id="rId6"/>
+    <sheet name="1ppb" sheetId="6" r:id="rId5"/>
+    <sheet name="Shotcrete Density" sheetId="5" r:id="rId6"/>
+    <sheet name="Shotcrete Hang" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="75">
   <si>
     <t>Decay</t>
   </si>
@@ -357,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -374,6 +375,7 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E56D091-102E-4A44-B40D-B7C123D87265}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2120,7 +2122,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2841,6 +2843,731 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB4BF7A-0142-9B4A-8871-96C42DF45FD4}">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31.5" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="32.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="C2" s="6">
+        <f>B2*($D$2/0.00000000000003)</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" ref="E2:E8" si="0">$F$2*C2</f>
+        <v>634619000000000</v>
+      </c>
+      <c r="F2" s="6">
+        <v>6.3461900000000002E+23</v>
+      </c>
+      <c r="G2" s="11">
+        <v>4.0815999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6">
+        <f>4.07056E-24</f>
+        <v>4.0705599999999999E-24</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:C8" si="1">B3*($D$2/0.00000000000003)</f>
+        <v>1.3568533333333334E-19</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
+        <v>86108.490554666671</v>
+      </c>
+      <c r="G3" s="11">
+        <v>5.5201500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6">
+        <f>2.11268E-26</f>
+        <v>2.1126800000000001E-26</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="1"/>
+        <v>7.0422666666666678E-22</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>446.91562297333343</v>
+      </c>
+      <c r="G4" s="11">
+        <v>5.7889214999999998</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.7546900000000003E-30</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2515633333333336E-25</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>7.9426587103666693E-2</v>
+      </c>
+      <c r="G5" s="11">
+        <v>6.4047409999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="13">
+        <v>9.8039200000000002E-33</v>
+      </c>
+      <c r="C6" s="13">
+        <f t="shared" si="1"/>
+        <v>3.2679733333333338E-28</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>2.073917968826667E-4</v>
+      </c>
+      <c r="G6" s="14">
+        <v>6.9063499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1.2898000000000001E-38</v>
+      </c>
+      <c r="C7" s="13">
+        <f t="shared" si="1"/>
+        <v>4.299333333333334E-34</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>2.728438620666667E-10</v>
+      </c>
+      <c r="G7" s="14">
+        <v>8.9541910999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13">
+        <f>2.45902E-28</f>
+        <v>2.4590199999999999E-28</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" si="1"/>
+        <v>8.1967333333333338E-24</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>5.2018027112666667</v>
+      </c>
+      <c r="G8" s="14">
+        <v>6.2072630000000002</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6">
+        <v>8.9999999999999995E-15</v>
+      </c>
+      <c r="C11" s="6">
+        <f>B11*($D$11/0.000000000000009)</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E11" s="6">
+        <f>$F$11*C11</f>
+        <v>634619000000000</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6.3461900000000002E+23</v>
+      </c>
+      <c r="G11" s="11">
+        <v>4.2699210000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6">
+        <f>4.94533E-19</f>
+        <v>4.9453300000000002E-19</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" ref="C12:C22" si="2">B12*($D$11/0.000000000000009)</f>
+        <v>5.4948111111111116E-14</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" ref="E12:E22" si="3">$F$11*C12</f>
+        <v>34871115325.222229</v>
+      </c>
+      <c r="G12" s="11">
+        <v>4.8575699999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6">
+        <f>1.51782E-19</f>
+        <v>1.5178200000000001E-19</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6864666666666669E-14</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="3"/>
+        <v>10702637895.333336</v>
+      </c>
+      <c r="G13" s="11">
+        <v>4.7700149999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6">
+        <f>3.22604E-21</f>
+        <v>3.22604E-21</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="2"/>
+        <v>3.5844888888888891E-16</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="3"/>
+        <v>227478475.41777781</v>
+      </c>
+      <c r="G14" s="11">
+        <v>4.87073</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2.1078800000000001E-26</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="2"/>
+        <v>2.3420888888888894E-21</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="3"/>
+        <v>1486.3341085777781</v>
+      </c>
+      <c r="G15" s="11">
+        <v>5.5904299999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1.9150299999999999E-35</v>
+      </c>
+      <c r="C16" s="13">
+        <f t="shared" si="2"/>
+        <v>2.1278111111111113E-30</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="13">
+        <f t="shared" si="3"/>
+        <v>1.3503493595222223E-6</v>
+      </c>
+      <c r="G16" s="14">
+        <v>6.8762999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1.1858500000000001E-29</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3176111111111114E-24</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.8361810457222224</v>
+      </c>
+      <c r="G17" s="11">
+        <v>6.1147590000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="13">
+        <v>1.04395E-35</v>
+      </c>
+      <c r="C18" s="13">
+        <f t="shared" si="2"/>
+        <v>1.1599444444444446E-30</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="3"/>
+        <v>7.3612278338888901E-7</v>
+      </c>
+      <c r="G18" s="14">
+        <v>7.8335460000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7.62767E-25</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="2"/>
+        <v>8.4751888888888893E-20</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="3"/>
+        <v>53785.158974777783</v>
+      </c>
+      <c r="G19" s="11">
+        <v>5.4075369999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="13">
+        <v>7.6275999999999997E-29</v>
+      </c>
+      <c r="C20" s="13">
+        <f t="shared" si="2"/>
+        <v>8.4751111111111123E-24</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="3"/>
+        <v>5.3784665382222228</v>
+      </c>
+      <c r="G20" s="14">
+        <v>5.6212999999999997</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2.7609400000000002E-26</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="2"/>
+        <v>3.0677111111111118E-21</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="3"/>
+        <v>1946.8277576222226</v>
+      </c>
+      <c r="G21" s="11">
+        <v>5.0365799999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="6">
+        <v>4.47794E-23</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="2"/>
+        <v>4.9754888888888893E-18</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="3"/>
+        <v>3157539.7831777781</v>
+      </c>
+      <c r="G22" s="11">
+        <v>3.7921999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6.4836000000000002E-17</v>
+      </c>
+      <c r="C26" s="6">
+        <f>B26*($D$26/6.4836E-17)</f>
+        <v>7.2040000000000004E-12</v>
+      </c>
+      <c r="D26" s="8">
+        <f>0.007204*D11</f>
+        <v>7.2040000000000004E-12</v>
+      </c>
+      <c r="E26" s="6">
+        <f>$F$26*C26</f>
+        <v>4571795276000</v>
+      </c>
+      <c r="F26" s="6">
+        <v>6.3461900000000002E+23</v>
+      </c>
+      <c r="G26" s="11">
+        <v>4.6781699999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="6">
+        <v>3.0157699999999998E-21</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" ref="C27:C37" si="4">B27*($D$26/6.4836E-17)</f>
+        <v>3.3508555555555554E-16</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" ref="E27:E37" si="5">$F$26*C27</f>
+        <v>212651660.1811111</v>
+      </c>
+      <c r="G27" s="11">
+        <v>5.1499800000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="6">
+        <v>4.6674600000000001E-27</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="4"/>
+        <v>5.1860666666666665E-22</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="5"/>
+        <v>329.11764419333332</v>
+      </c>
+      <c r="G28" s="11">
+        <v>6.1466010000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="6">
+        <v>2.0074E-24</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="4"/>
+        <v>2.2304444444444444E-19</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="5"/>
+        <v>141548.2422888889</v>
+      </c>
+      <c r="G29" s="11">
+        <v>5.0422713999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="6">
+        <v>2.8817300000000002E-27</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="4"/>
+        <v>3.2019222222222224E-22</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="5"/>
+        <v>203.20006787444447</v>
+      </c>
+      <c r="G30" s="11">
+        <v>5.9789921000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="6">
+        <v>5.32606E-32</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="4"/>
+        <v>5.9178444444444445E-27</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="5"/>
+        <v>3.755576523488889E-3</v>
+      </c>
+      <c r="G31" s="11">
+        <v>5.5613000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="13">
+        <v>1.15793E-32</v>
+      </c>
+      <c r="C32" s="13">
+        <f t="shared" si="4"/>
+        <v>1.2865888888888888E-27</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="5"/>
+        <v>8.1649375407777771E-4</v>
+      </c>
+      <c r="G32" s="14">
+        <v>6.9462299999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="6">
+        <v>1.3557199999999999E-35</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="4"/>
+        <v>1.5063555555555554E-30</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="5"/>
+        <v>9.5596185631111091E-7</v>
+      </c>
+      <c r="G33" s="11">
+        <v>6.3425000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="13">
+        <v>2.9209100000000002E-37</v>
+      </c>
+      <c r="C34" s="13">
+        <f t="shared" si="4"/>
+        <v>3.2454555555555558E-32</v>
+      </c>
+      <c r="E34" s="13">
+        <f t="shared" si="5"/>
+        <v>2.0596277592111113E-8</v>
+      </c>
+      <c r="G34" s="14">
+        <v>8.1783999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="13">
+        <v>5.1875399999999997E-36</v>
+      </c>
+      <c r="C35" s="13">
+        <f t="shared" si="4"/>
+        <v>5.7639333333333326E-31</v>
+      </c>
+      <c r="E35" s="13">
+        <f t="shared" si="5"/>
+        <v>3.6579016080666663E-7</v>
+      </c>
+      <c r="G35" s="14">
+        <v>7.5263799999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="13">
+        <v>1.50413E-33</v>
+      </c>
+      <c r="C36" s="13">
+        <f t="shared" si="4"/>
+        <v>1.6712555555555556E-28</v>
+      </c>
+      <c r="E36" s="13">
+        <f t="shared" si="5"/>
+        <v>1.0606105294111112E-4</v>
+      </c>
+      <c r="G36" s="14">
+        <v>7.5946499999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="13">
+        <v>3.7490899999999998E-31</v>
+      </c>
+      <c r="C37" s="13">
+        <f t="shared" si="4"/>
+        <v>4.1656555555555551E-26</v>
+      </c>
+      <c r="E37" s="13">
+        <f t="shared" si="5"/>
+        <v>2.643604163011111E-2</v>
+      </c>
+      <c r="G37" s="14">
+        <v>6.7504499999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C0C8FF-B22E-AA44-AF26-339606D55407}">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -3317,723 +4044,129 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB4BF7A-0142-9B4A-8871-96C42DF45FD4}">
-  <dimension ref="A1:K37"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A89027-C8C3-1B4E-B23A-0C8C2B287B0A}">
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="31.5" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="32.83203125" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="1" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3.3300000000000003E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>9.7799999999999992E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4.86E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="6">
-        <v>2.9999999999999998E-14</v>
-      </c>
-      <c r="C2" s="6">
-        <f>B2*($D$2/0.00000000000003)</f>
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="E2" s="6">
-        <f t="shared" ref="E2:E8" si="0">$F$2*C2</f>
-        <v>634619000000000</v>
-      </c>
-      <c r="F2" s="6">
-        <v>6.3461900000000002E+23</v>
-      </c>
-      <c r="G2" s="11">
-        <v>4.0815999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6">
-        <f>4.07056E-24</f>
-        <v>4.0705599999999999E-24</v>
-      </c>
-      <c r="C3" s="6">
-        <f t="shared" ref="C3:C8" si="1">B3*($D$2/0.00000000000003)</f>
-        <v>1.3568533333333334E-19</v>
-      </c>
-      <c r="E3" s="6">
-        <f t="shared" si="0"/>
-        <v>86108.490554666671</v>
-      </c>
-      <c r="G3" s="11">
-        <v>5.5201500000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="6">
-        <f>2.11268E-26</f>
-        <v>2.1126800000000001E-26</v>
-      </c>
-      <c r="C4" s="6">
-        <f t="shared" si="1"/>
-        <v>7.0422666666666678E-22</v>
-      </c>
-      <c r="E4" s="6">
-        <f t="shared" si="0"/>
-        <v>446.91562297333343</v>
-      </c>
-      <c r="G4" s="11">
-        <v>5.7889214999999998</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B7" s="2">
+        <v>2.2399999999999998E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>14</v>
       </c>
-      <c r="B5" s="6">
-        <v>3.7546900000000003E-30</v>
-      </c>
-      <c r="C5" s="6">
-        <f t="shared" si="1"/>
-        <v>1.2515633333333336E-25</v>
-      </c>
-      <c r="E5" s="6">
-        <f t="shared" si="0"/>
-        <v>7.9426587103666693E-2</v>
-      </c>
-      <c r="G5" s="11">
-        <v>6.4047409999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="13">
-        <v>9.8039200000000002E-33</v>
-      </c>
-      <c r="C6" s="13">
-        <f t="shared" si="1"/>
-        <v>3.2679733333333338E-28</v>
-      </c>
-      <c r="E6" s="13">
-        <f t="shared" si="0"/>
-        <v>2.073917968826667E-4</v>
-      </c>
-      <c r="G6" s="14">
-        <v>6.9063499999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="13">
-        <v>1.2898000000000001E-38</v>
-      </c>
-      <c r="C7" s="13">
-        <f t="shared" si="1"/>
-        <v>4.299333333333334E-34</v>
-      </c>
-      <c r="E7" s="13">
-        <f t="shared" si="0"/>
-        <v>2.728438620666667E-10</v>
-      </c>
-      <c r="G7" s="14">
-        <v>8.9541910999999992</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="13">
-        <f>2.45902E-28</f>
-        <v>2.4590199999999999E-28</v>
-      </c>
-      <c r="C8" s="13">
-        <f t="shared" si="1"/>
-        <v>8.1967333333333338E-24</v>
-      </c>
-      <c r="E8" s="13">
-        <f t="shared" si="0"/>
-        <v>5.2018027112666667</v>
-      </c>
-      <c r="G8" s="14">
-        <v>6.2072630000000002</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="6">
-        <v>8.9999999999999995E-15</v>
-      </c>
-      <c r="C11" s="6">
-        <f>B11*($D$11/0.000000000000009)</f>
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="E11" s="6">
-        <f>$F$11*C11</f>
-        <v>634619000000000</v>
-      </c>
-      <c r="F11" s="6">
-        <v>6.3461900000000002E+23</v>
-      </c>
-      <c r="G11" s="11">
-        <v>4.2699210000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B8" s="2">
+        <v>9.9299999999999996E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>19</v>
       </c>
-      <c r="B12" s="6">
-        <f>4.94533E-19</f>
-        <v>4.9453300000000002E-19</v>
-      </c>
-      <c r="C12" s="6">
-        <f t="shared" ref="C12:C22" si="2">B12*($D$11/0.000000000000009)</f>
-        <v>5.4948111111111116E-14</v>
-      </c>
-      <c r="E12" s="6">
-        <f t="shared" ref="E12:E22" si="3">$F$11*C12</f>
-        <v>34871115325.222229</v>
-      </c>
-      <c r="G12" s="11">
-        <v>4.8575699999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B9" s="2">
+        <v>4.4999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>20</v>
       </c>
-      <c r="B13" s="6">
-        <f>1.51782E-19</f>
-        <v>1.5178200000000001E-19</v>
-      </c>
-      <c r="C13" s="6">
-        <f t="shared" si="2"/>
-        <v>1.6864666666666669E-14</v>
-      </c>
-      <c r="E13" s="6">
-        <f t="shared" si="3"/>
-        <v>10702637895.333336</v>
-      </c>
-      <c r="G13" s="11">
-        <v>4.7700149999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="6">
-        <f>3.22604E-21</f>
-        <v>3.22604E-21</v>
-      </c>
-      <c r="C14" s="6">
-        <f t="shared" si="2"/>
-        <v>3.5844888888888891E-16</v>
-      </c>
-      <c r="E14" s="6">
-        <f t="shared" si="3"/>
-        <v>227478475.41777781</v>
-      </c>
-      <c r="G14" s="11">
-        <v>4.87073</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="6">
-        <v>2.1078800000000001E-26</v>
-      </c>
-      <c r="C15" s="6">
-        <f t="shared" si="2"/>
-        <v>2.3420888888888894E-21</v>
-      </c>
-      <c r="E15" s="6">
-        <f t="shared" si="3"/>
-        <v>1486.3341085777781</v>
-      </c>
-      <c r="G15" s="11">
-        <v>5.5904299999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="13">
-        <v>1.9150299999999999E-35</v>
-      </c>
-      <c r="C16" s="13">
-        <f t="shared" si="2"/>
-        <v>2.1278111111111113E-30</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="13">
-        <f t="shared" si="3"/>
-        <v>1.3503493595222223E-6</v>
-      </c>
-      <c r="G16" s="14">
-        <v>6.8762999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1.1858500000000001E-29</v>
-      </c>
-      <c r="C17" s="6">
-        <f t="shared" si="2"/>
-        <v>1.3176111111111114E-24</v>
-      </c>
-      <c r="E17" s="6">
-        <f t="shared" si="3"/>
-        <v>0.8361810457222224</v>
-      </c>
-      <c r="G17" s="11">
-        <v>6.1147590000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="B10" s="2">
+        <v>2.3800000000000002E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2">
+        <v>6.7299999999999996E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>26</v>
       </c>
-      <c r="B18" s="13">
-        <v>1.04395E-35</v>
-      </c>
-      <c r="C18" s="13">
-        <f t="shared" si="2"/>
-        <v>1.1599444444444446E-30</v>
-      </c>
-      <c r="E18" s="13">
-        <f t="shared" si="3"/>
-        <v>7.3612278338888901E-7</v>
-      </c>
-      <c r="G18" s="14">
-        <v>7.8335460000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="6">
-        <v>7.62767E-25</v>
-      </c>
-      <c r="C19" s="6">
-        <f t="shared" si="2"/>
-        <v>8.4751888888888893E-20</v>
-      </c>
-      <c r="E19" s="6">
-        <f t="shared" si="3"/>
-        <v>53785.158974777783</v>
-      </c>
-      <c r="G19" s="11">
-        <v>5.4075369999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="13">
-        <v>7.6275999999999997E-29</v>
-      </c>
-      <c r="C20" s="13">
-        <f t="shared" si="2"/>
-        <v>8.4751111111111123E-24</v>
-      </c>
-      <c r="E20" s="13">
-        <f t="shared" si="3"/>
-        <v>5.3784665382222228</v>
-      </c>
-      <c r="G20" s="14">
-        <v>5.6212999999999997</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="6">
-        <v>2.7609400000000002E-26</v>
-      </c>
-      <c r="C21" s="6">
-        <f t="shared" si="2"/>
-        <v>3.0677111111111118E-21</v>
-      </c>
-      <c r="E21" s="6">
-        <f t="shared" si="3"/>
-        <v>1946.8277576222226</v>
-      </c>
-      <c r="G21" s="11">
-        <v>5.0365799999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="6">
-        <v>4.47794E-23</v>
-      </c>
-      <c r="C22" s="6">
-        <f t="shared" si="2"/>
-        <v>4.9754888888888893E-18</v>
-      </c>
-      <c r="E22" s="6">
-        <f t="shared" si="3"/>
-        <v>3157539.7831777781</v>
-      </c>
-      <c r="G22" s="11">
-        <v>3.7921999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="6">
-        <v>6.4836000000000002E-17</v>
-      </c>
-      <c r="C26" s="6">
-        <f>B26*($D$26/6.4836E-17)</f>
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="D26" s="8">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="E26" s="6">
-        <f>$F$26*C26</f>
-        <v>634619000000000</v>
-      </c>
-      <c r="F26" s="6">
-        <v>6.3461900000000002E+23</v>
-      </c>
-      <c r="G26" s="11">
-        <v>4.6781699999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="6">
-        <v>3.0157699999999998E-21</v>
-      </c>
-      <c r="C27" s="6">
-        <f t="shared" ref="C27:C37" si="4">B27*($D$26/6.4836E-17)</f>
-        <v>4.6513819483003271E-14</v>
-      </c>
-      <c r="E27" s="6">
-        <f t="shared" ref="E27:E37" si="5">$F$26*C27</f>
-        <v>29518553606.484055</v>
-      </c>
-      <c r="G27" s="11">
-        <v>5.1499800000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="6">
-        <v>4.6674600000000001E-27</v>
-      </c>
-      <c r="C28" s="6">
-        <f t="shared" si="4"/>
-        <v>7.1988709975939301E-20</v>
-      </c>
-      <c r="E28" s="6">
-        <f t="shared" si="5"/>
-        <v>45685.403136220622</v>
-      </c>
-      <c r="G28" s="11">
-        <v>6.1466010000000004</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="6">
-        <v>2.0074E-24</v>
-      </c>
-      <c r="C29" s="6">
-        <f t="shared" si="4"/>
-        <v>3.0961194398173858E-17</v>
-      </c>
-      <c r="E29" s="6">
-        <f t="shared" si="5"/>
-        <v>19648562.227774695</v>
-      </c>
-      <c r="G29" s="11">
-        <v>5.0422713999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="6">
-        <v>2.8817300000000002E-27</v>
-      </c>
-      <c r="C30" s="6">
-        <f t="shared" si="4"/>
-        <v>4.4446449503362333E-20</v>
-      </c>
-      <c r="E30" s="6">
-        <f t="shared" si="5"/>
-        <v>28206.5613373743</v>
-      </c>
-      <c r="G30" s="11">
-        <v>5.9789921000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="6">
-        <v>5.32606E-32</v>
-      </c>
-      <c r="C31" s="6">
-        <f t="shared" si="4"/>
-        <v>8.2146646924548096E-25</v>
-      </c>
-      <c r="E31" s="6">
-        <f t="shared" si="5"/>
-        <v>0.52131822924609794</v>
-      </c>
-      <c r="G31" s="11">
-        <v>5.5613000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="13">
-        <v>1.15793E-32</v>
-      </c>
-      <c r="C32" s="13">
-        <f t="shared" si="4"/>
-        <v>1.7859368252205565E-25</v>
-      </c>
-      <c r="E32" s="13">
-        <f t="shared" si="5"/>
-        <v>0.11333894420846444</v>
-      </c>
-      <c r="G32" s="14">
-        <v>6.9462299999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="6">
-        <v>1.3557199999999999E-35</v>
-      </c>
-      <c r="C33" s="6">
-        <f t="shared" si="4"/>
-        <v>2.0909988278117094E-28</v>
-      </c>
-      <c r="E33" s="6">
-        <f t="shared" si="5"/>
-        <v>1.3269875851070392E-4</v>
-      </c>
-      <c r="G33" s="11">
-        <v>6.3425000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="13">
-        <v>2.9209100000000002E-37</v>
-      </c>
-      <c r="C34" s="13">
-        <f t="shared" si="4"/>
-        <v>4.5050743414152638E-30</v>
-      </c>
-      <c r="E34" s="13">
-        <f t="shared" si="5"/>
-        <v>2.8590057734746135E-6</v>
-      </c>
-      <c r="G34" s="14">
-        <v>8.1783999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="13">
-        <v>5.1875399999999997E-36</v>
-      </c>
-      <c r="C35" s="13">
-        <f t="shared" si="4"/>
-        <v>8.0010179529890804E-29</v>
-      </c>
-      <c r="E35" s="13">
-        <f t="shared" si="5"/>
-        <v>5.0775980123079771E-5</v>
-      </c>
-      <c r="G35" s="14">
-        <v>7.5263799999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="13">
-        <v>1.50413E-33</v>
-      </c>
-      <c r="C36" s="13">
-        <f t="shared" si="4"/>
-        <v>2.3198994385835032E-26</v>
-      </c>
-      <c r="E36" s="13">
-        <f t="shared" si="5"/>
-        <v>1.4722522618144242E-2</v>
-      </c>
-      <c r="G36" s="14">
-        <v>7.5946499999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="13">
-        <v>3.7490899999999998E-31</v>
-      </c>
-      <c r="C37" s="13">
-        <f t="shared" si="4"/>
-        <v>5.782420260349189E-24</v>
-      </c>
-      <c r="E37" s="13">
-        <f t="shared" si="5"/>
-        <v>3.6696337632025422</v>
-      </c>
-      <c r="G37" s="14">
-        <v>6.7504499999999998</v>
+      <c r="B12" s="2">
+        <v>4.5399999999999998E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="16">
+        <f>SUM(B2:B12)</f>
+        <v>4.7418600000000005E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ANV] updated the tapes for 1ppb
</commit_message>
<xml_diff>
--- a/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
+++ b/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC1FB7D-2C08-3C40-9487-E93E023EB3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E0026F-E943-BD4C-81C7-DDAF6BBCCB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="7" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
@@ -4407,6 +4407,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>7.022728404246925E-4</v>
+      </c>
       <c r="C4" s="22">
         <v>13</v>
       </c>
@@ -4417,16 +4420,16 @@
         <v>1.6</v>
       </c>
       <c r="F4" s="25">
-        <f>(D4+E4)/200</f>
-        <v>1.2800000000000001E-2</v>
+        <f>B4*(D4+E4)/200</f>
+        <v>8.9890923574360637E-6</v>
       </c>
       <c r="G4" s="25">
-        <f>D4/100</f>
-        <v>9.5999999999999992E-3</v>
+        <f>B4*D4/100</f>
+        <v>6.7418192680770474E-6</v>
       </c>
       <c r="H4" s="25">
-        <f>E4/100</f>
-        <v>1.6E-2</v>
+        <f>B4*E4/100</f>
+        <v>1.1236365446795079E-5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -4441,6 +4444,9 @@
       <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>0.63266447300513629</v>
+      </c>
       <c r="C6" s="22">
         <v>17</v>
       </c>
@@ -4451,19 +4457,22 @@
         <v>0.04</v>
       </c>
       <c r="F6" s="25">
-        <f t="shared" ref="F5:F36" si="0">(D6+E6)/200</f>
-        <v>3.835E-4</v>
+        <f t="shared" ref="F5:F36" si="0">B6*(D6+E6)/200</f>
+        <v>2.4262682539746976E-4</v>
       </c>
       <c r="G6" s="25">
-        <f t="shared" ref="G5:G36" si="1">D6/100</f>
-        <v>3.6700000000000003E-4</v>
+        <f t="shared" ref="G5:G36" si="1">B6*D6/100</f>
+        <v>2.3218786159288506E-4</v>
       </c>
       <c r="H6" s="25">
-        <f t="shared" ref="H5:H36" si="2">E6/100</f>
-        <v>4.0000000000000002E-4</v>
+        <f t="shared" ref="H5:H36" si="2">B6*E6/100</f>
+        <v>2.5306578920205453E-4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>0.63266447300513629</v>
+      </c>
       <c r="C7" s="22">
         <v>18</v>
       </c>
@@ -4475,15 +4484,15 @@
       </c>
       <c r="F7" s="25">
         <f t="shared" si="0"/>
-        <v>2.0449999999999999E-3</v>
+        <v>1.293798847295504E-3</v>
       </c>
       <c r="G7" s="25">
         <f t="shared" si="1"/>
-        <v>1.8699999999999999E-3</v>
+        <v>1.1830825645196049E-3</v>
       </c>
       <c r="H7" s="25">
         <f t="shared" si="2"/>
-        <v>2.2200000000000002E-3</v>
+        <v>1.4045151300714027E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -4498,6 +4507,9 @@
       <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>2.063825428636017E-2</v>
+      </c>
       <c r="C9" s="22">
         <v>23</v>
       </c>
@@ -4509,15 +4521,15 @@
       </c>
       <c r="F9" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.063825428636017E-2</v>
       </c>
       <c r="G9" s="25">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.063825428636017E-2</v>
       </c>
       <c r="H9" s="25">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.063825428636017E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -4532,6 +4544,9 @@
       <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>1.023791290051672E-2</v>
+      </c>
       <c r="C11" s="22">
         <v>24</v>
       </c>
@@ -4543,18 +4558,21 @@
       </c>
       <c r="F11" s="25">
         <f t="shared" si="0"/>
-        <v>0.78965000000000007</v>
+        <v>8.0843679218930292E-3</v>
       </c>
       <c r="G11" s="25">
         <f t="shared" si="1"/>
-        <v>0.78879999999999995</v>
+        <v>8.0756656959275891E-3</v>
       </c>
       <c r="H11" s="25">
         <f t="shared" si="2"/>
-        <v>0.79049999999999998</v>
+        <v>8.0930701478584659E-3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>1.023791290051672E-2</v>
+      </c>
       <c r="C12" s="22">
         <v>25</v>
       </c>
@@ -4566,18 +4584,21 @@
       </c>
       <c r="F12" s="25">
         <f t="shared" si="0"/>
-        <v>0.10010999999999999</v>
+        <v>1.0249174604707288E-3</v>
       </c>
       <c r="G12" s="25">
         <f t="shared" si="1"/>
-        <v>9.9879999999999997E-2</v>
+        <v>1.0225627405036101E-3</v>
       </c>
       <c r="H12" s="25">
         <f t="shared" si="2"/>
-        <v>0.10034000000000001</v>
+        <v>1.0272721804378477E-3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>1.023791290051672E-2</v>
+      </c>
       <c r="C13" s="22">
         <v>26</v>
       </c>
@@ -4589,15 +4610,15 @@
       </c>
       <c r="F13" s="25">
         <f t="shared" si="0"/>
-        <v>0.11025</v>
+        <v>1.1287298972819685E-3</v>
       </c>
       <c r="G13" s="25">
         <f t="shared" si="1"/>
-        <v>0.1096</v>
+        <v>1.1220752538966326E-3</v>
       </c>
       <c r="H13" s="25">
         <f t="shared" si="2"/>
-        <v>0.1109</v>
+        <v>1.1353845406673042E-3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -4612,6 +4633,9 @@
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>4.720578993057023E-2</v>
+      </c>
       <c r="C15" s="22">
         <v>27</v>
       </c>
@@ -4623,15 +4647,15 @@
       </c>
       <c r="F15" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4.720578993057023E-2</v>
       </c>
       <c r="G15" s="25">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4.720578993057023E-2</v>
       </c>
       <c r="H15" s="25">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4.720578993057023E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -4646,6 +4670,9 @@
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>0.20948218342998465</v>
+      </c>
       <c r="C17" s="22">
         <v>28</v>
       </c>
@@ -4657,18 +4684,21 @@
       </c>
       <c r="F17" s="25">
         <f t="shared" si="0"/>
-        <v>0.92254500000000006</v>
+        <v>0.19325674091241521</v>
       </c>
       <c r="G17" s="25">
         <f t="shared" si="1"/>
-        <v>0.92191000000000001</v>
+        <v>0.19312371972593717</v>
       </c>
       <c r="H17" s="25">
         <f t="shared" si="2"/>
-        <v>0.92318</v>
+        <v>0.19338976209889322</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>0.20948218342998465</v>
+      </c>
       <c r="C18" s="22">
         <v>29</v>
       </c>
@@ -4680,18 +4710,21 @@
       </c>
       <c r="F18" s="25">
         <f t="shared" si="0"/>
-        <v>4.6719999999999998E-2</v>
+        <v>9.7870076098488818E-3</v>
       </c>
       <c r="G18" s="25">
         <f t="shared" si="1"/>
-        <v>4.6449999999999998E-2</v>
+        <v>9.7304474203227867E-3</v>
       </c>
       <c r="H18" s="25">
         <f t="shared" si="2"/>
-        <v>4.6989999999999997E-2</v>
+        <v>9.8435677993749787E-3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>0.20948218342998465</v>
+      </c>
       <c r="C19" s="22">
         <v>30</v>
       </c>
@@ -4703,15 +4736,15 @@
       </c>
       <c r="F19" s="25">
         <f t="shared" si="0"/>
-        <v>3.0735000000000002E-2</v>
+        <v>6.4384349077205782E-3</v>
       </c>
       <c r="G19" s="25">
         <f t="shared" si="1"/>
-        <v>3.0369999999999998E-2</v>
+        <v>6.3619739107686332E-3</v>
       </c>
       <c r="H19" s="25">
         <f t="shared" si="2"/>
-        <v>3.1099999999999999E-2</v>
+        <v>6.5148959046725215E-3</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -4726,6 +4759,9 @@
       <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>9.492483299759916E-3</v>
+      </c>
       <c r="C21" s="22">
         <v>39</v>
       </c>
@@ -4737,18 +4773,21 @@
       </c>
       <c r="F21" s="25">
         <f t="shared" si="0"/>
-        <v>0.93258099999999999</v>
+        <v>8.8525095681734021E-3</v>
       </c>
       <c r="G21" s="25">
         <f t="shared" si="1"/>
-        <v>0.93258099999999999</v>
+        <v>8.8525095681734021E-3</v>
       </c>
       <c r="H21" s="25">
         <f t="shared" si="2"/>
-        <v>0.93258099999999999</v>
+        <v>8.8525095681734021E-3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>9.492483299759916E-3</v>
+      </c>
       <c r="C22" s="22">
         <v>40</v>
       </c>
@@ -4760,18 +4799,21 @@
       </c>
       <c r="F22" s="25">
         <f t="shared" si="0"/>
-        <v>1.17E-4</v>
+        <v>1.1106205460719101E-6</v>
       </c>
       <c r="G22" s="25">
         <f t="shared" si="1"/>
-        <v>1.17E-4</v>
+        <v>1.1106205460719101E-6</v>
       </c>
       <c r="H22" s="25">
         <f t="shared" si="2"/>
-        <v>1.17E-4</v>
+        <v>1.1106205460719101E-6</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>9.492483299759916E-3</v>
+      </c>
       <c r="C23" s="22">
         <v>41</v>
       </c>
@@ -4783,15 +4825,15 @@
       </c>
       <c r="F23" s="25">
         <f t="shared" si="0"/>
-        <v>6.7302000000000001E-2</v>
+        <v>6.3886311104044196E-4</v>
       </c>
       <c r="G23" s="25">
         <f t="shared" si="1"/>
-        <v>6.7302000000000001E-2</v>
+        <v>6.3886311104044196E-4</v>
       </c>
       <c r="H23" s="25">
         <f t="shared" si="2"/>
-        <v>6.7302000000000001E-2</v>
+        <v>6.3886311104044196E-4</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -4806,6 +4848,9 @@
       <c r="H24" s="25"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>5.0195800241836508E-2</v>
+      </c>
       <c r="C25" s="22">
         <v>42</v>
       </c>
@@ -4817,18 +4862,21 @@
       </c>
       <c r="F25" s="25">
         <f t="shared" si="0"/>
-        <v>6.4700000000000001E-3</v>
+        <v>3.2476682756468219E-4</v>
       </c>
       <c r="G25" s="25">
         <f t="shared" si="1"/>
-        <v>6.4700000000000001E-3</v>
+        <v>3.2476682756468219E-4</v>
       </c>
       <c r="H25" s="25">
         <f t="shared" si="2"/>
-        <v>6.4700000000000001E-3</v>
+        <v>3.2476682756468219E-4</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>5.0195800241836508E-2</v>
+      </c>
       <c r="C26" s="22">
         <v>43</v>
       </c>
@@ -4840,18 +4888,21 @@
       </c>
       <c r="F26" s="25">
         <f t="shared" si="0"/>
-        <v>1.3500000000000001E-3</v>
+        <v>6.7764330326479288E-5</v>
       </c>
       <c r="G26" s="25">
         <f t="shared" si="1"/>
-        <v>1.3500000000000001E-3</v>
+        <v>6.7764330326479288E-5</v>
       </c>
       <c r="H26" s="25">
         <f t="shared" si="2"/>
-        <v>1.3500000000000001E-3</v>
+        <v>6.7764330326479288E-5</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>5.0195800241836508E-2</v>
+      </c>
       <c r="C27" s="22">
         <v>44</v>
       </c>
@@ -4863,18 +4914,21 @@
       </c>
       <c r="F27" s="25">
         <f t="shared" si="0"/>
-        <v>2.086E-2</v>
+        <v>1.0470843930447094E-3</v>
       </c>
       <c r="G27" s="25">
         <f t="shared" si="1"/>
-        <v>2.086E-2</v>
+        <v>1.0470843930447094E-3</v>
       </c>
       <c r="H27" s="25">
         <f t="shared" si="2"/>
-        <v>2.086E-2</v>
+        <v>1.0470843930447094E-3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>5.0195800241836508E-2</v>
+      </c>
       <c r="C28" s="22">
         <v>46</v>
       </c>
@@ -4886,18 +4940,21 @@
       </c>
       <c r="F28" s="25">
         <f t="shared" si="0"/>
-        <v>4.0000000000000003E-5</v>
+        <v>2.0078320096734603E-6</v>
       </c>
       <c r="G28" s="25">
         <f t="shared" si="1"/>
-        <v>4.0000000000000003E-5</v>
+        <v>2.0078320096734603E-6</v>
       </c>
       <c r="H28" s="25">
         <f t="shared" si="2"/>
-        <v>4.0000000000000003E-5</v>
+        <v>2.0078320096734603E-6</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>5.0195800241836508E-2</v>
+      </c>
       <c r="C29" s="22">
         <v>48</v>
       </c>
@@ -4909,15 +4966,15 @@
       </c>
       <c r="F29" s="25">
         <f t="shared" si="0"/>
-        <v>1.8699999999999999E-3</v>
+        <v>9.3866146452234263E-5</v>
       </c>
       <c r="G29" s="25">
         <f t="shared" si="1"/>
-        <v>1.8699999999999999E-3</v>
+        <v>9.3866146452234263E-5</v>
       </c>
       <c r="H29" s="25">
         <f t="shared" si="2"/>
-        <v>1.8699999999999999E-3</v>
+        <v>9.3866146452234263E-5</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -4932,6 +4989,9 @@
       <c r="H30" s="25"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>1.4202133142682343E-3</v>
+      </c>
       <c r="C31" s="22">
         <v>55</v>
       </c>
@@ -4943,15 +5003,15 @@
       </c>
       <c r="F31" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.4202133142682343E-3</v>
       </c>
       <c r="G31" s="25">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.4202133142682343E-3</v>
       </c>
       <c r="H31" s="25">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.4202133142682343E-3</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -4966,6 +5026,9 @@
       <c r="H32" s="25"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>9.5912336284833428E-3</v>
+      </c>
       <c r="C33" s="22">
         <v>54</v>
       </c>
@@ -4977,18 +5040,21 @@
       </c>
       <c r="F33" s="25">
         <f t="shared" si="0"/>
-        <v>5.8449999999999995E-2</v>
+        <v>5.6060760558485133E-4</v>
       </c>
       <c r="G33" s="25">
         <f t="shared" si="1"/>
-        <v>5.8449999999999995E-2</v>
+        <v>5.6060760558485133E-4</v>
       </c>
       <c r="H33" s="25">
         <f t="shared" si="2"/>
-        <v>5.8449999999999995E-2</v>
+        <v>5.6060760558485133E-4</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>9.5912336284833428E-3</v>
+      </c>
       <c r="C34" s="22">
         <v>56</v>
       </c>
@@ -5000,18 +5066,21 @@
       </c>
       <c r="F34" s="25">
         <f t="shared" si="0"/>
-        <v>0.91754000000000002</v>
+        <v>8.8003405034786063E-3</v>
       </c>
       <c r="G34" s="25">
         <f t="shared" si="1"/>
-        <v>0.91754000000000002</v>
+        <v>8.8003405034786063E-3</v>
       </c>
       <c r="H34" s="25">
         <f t="shared" si="2"/>
-        <v>0.91754000000000002</v>
+        <v>8.8003405034786063E-3</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>9.5912336284833428E-3</v>
+      </c>
       <c r="C35" s="22">
         <v>57</v>
       </c>
@@ -5023,18 +5092,21 @@
       </c>
       <c r="F35" s="25">
         <f t="shared" si="0"/>
-        <v>2.1190000000000001E-2</v>
+        <v>2.0323824058756206E-4</v>
       </c>
       <c r="G35" s="25">
         <f t="shared" si="1"/>
-        <v>2.1190000000000001E-2</v>
+        <v>2.0323824058756206E-4</v>
       </c>
       <c r="H35" s="25">
         <f t="shared" si="2"/>
-        <v>2.1190000000000001E-2</v>
+        <v>2.0323824058756206E-4</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>9.5912336284833428E-3</v>
+      </c>
       <c r="C36" s="22">
         <v>58</v>
       </c>
@@ -5046,15 +5118,15 @@
       </c>
       <c r="F36" s="25">
         <f t="shared" si="0"/>
-        <v>2.8199999999999996E-3</v>
+        <v>2.7047278832323025E-5</v>
       </c>
       <c r="G36" s="25">
         <f t="shared" si="1"/>
-        <v>2.8199999999999996E-3</v>
+        <v>2.7047278832323025E-5</v>
       </c>
       <c r="H36" s="25">
         <f t="shared" si="2"/>
-        <v>2.8199999999999996E-3</v>
+        <v>2.7047278832323025E-5</v>
       </c>
     </row>
     <row r="37" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[ANV] updated decay chains
</commit_message>
<xml_diff>
--- a/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
+++ b/SOURCES/sources_running/data/raw_sources_IO/decay_chains_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E0026F-E943-BD4C-81C7-DDAF6BBCCB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E261B43F-3B59-9B43-B643-4CAA6E2C2A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="7" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="85">
   <si>
     <t>Decay</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>Upper (frac)</t>
+  </si>
+  <si>
+    <t>Middle (frac): Hang's Normalization</t>
   </si>
 </sst>
 </file>
@@ -4088,7 +4091,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4347,10 +4350,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FFCC7E-9834-0644-A762-CED2A17019DD}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4362,9 +4365,10 @@
     <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="26.1640625" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>44</v>
       </c>
@@ -4389,8 +4393,11 @@
       <c r="H1" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4398,7 +4405,7 @@
         <v>8.3693831226593299E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
@@ -4406,7 +4413,7 @@
         <v>7.022728404246925E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>7.022728404246925E-4</v>
       </c>
@@ -4431,8 +4438,12 @@
         <f>B4*E4/100</f>
         <v>1.1236365446795079E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="25">
+        <f>F4*'Shotcrete Hang'!$B$13</f>
+        <v>4.262501748603178E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
@@ -4442,8 +4453,9 @@
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>0.63266447300513629</v>
       </c>
@@ -4468,8 +4480,12 @@
         <f t="shared" ref="H5:H36" si="2">B6*E6/100</f>
         <v>2.5306578920205453E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="25">
+        <f>F6*'Shotcrete Hang'!$B$13</f>
+        <v>1.1505024382792461E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>0.63266447300513629</v>
       </c>
@@ -4494,8 +4510,12 @@
         <f t="shared" si="2"/>
         <v>1.4045151300714027E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="25">
+        <f>F7*'Shotcrete Hang'!$B$13</f>
+        <v>6.1350130020366598E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>11</v>
       </c>
@@ -4505,8 +4525,9 @@
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>2.063825428636017E-2</v>
       </c>
@@ -4531,8 +4552,12 @@
         <f t="shared" si="2"/>
         <v>2.063825428636017E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="25">
+        <f>F9*'Shotcrete Hang'!$B$13</f>
+        <v>9.7863712470319837E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>12</v>
       </c>
@@ -4542,8 +4567,9 @@
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>1.023791290051672E-2</v>
       </c>
@@ -4568,8 +4594,12 @@
         <f t="shared" si="2"/>
         <v>8.0930701478584659E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="25">
+        <f>F11*'Shotcrete Hang'!$B$13</f>
+        <v>3.8334940874107685E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>1.023791290051672E-2</v>
       </c>
@@ -4594,8 +4624,12 @@
         <f t="shared" si="2"/>
         <v>1.0272721804378477E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="25">
+        <f>F12*'Shotcrete Hang'!$B$13</f>
+        <v>4.8600151091077308E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>1.023791290051672E-2</v>
       </c>
@@ -4620,8 +4654,12 @@
         <f t="shared" si="2"/>
         <v>1.1353845406673042E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="25">
+        <f>F13*'Shotcrete Hang'!$B$13</f>
+        <v>5.3522791507254758E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4631,8 +4669,9 @@
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>4.720578993057023E-2</v>
       </c>
@@ -4657,8 +4696,12 @@
         <f t="shared" si="2"/>
         <v>4.720578993057023E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="25">
+        <f>F15*'Shotcrete Hang'!$B$13</f>
+        <v>2.2384324704017378E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4668,8 +4711,9 @@
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>0.20948218342998465</v>
       </c>
@@ -4694,8 +4738,12 @@
         <f t="shared" si="2"/>
         <v>0.19338976209889322</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="25">
+        <f>F17*'Shotcrete Hang'!$B$13</f>
+        <v>9.163964094629452E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>0.20948218342998465</v>
       </c>
@@ -4720,8 +4768,12 @@
         <f t="shared" si="2"/>
         <v>9.8435677993749787E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="25">
+        <f>F18*'Shotcrete Hang'!$B$13</f>
+        <v>4.6408619904838026E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>0.20948218342998465</v>
       </c>
@@ -4746,8 +4798,12 @@
         <f t="shared" si="2"/>
         <v>6.5148959046725215E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="25">
+        <f>F19*'Shotcrete Hang'!$B$13</f>
+        <v>3.0530156951523907E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4757,8 +4813,9 @@
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="25"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>9.492483299759916E-3</v>
       </c>
@@ -4783,8 +4840,12 @@
         <f t="shared" si="2"/>
         <v>8.8525095681734021E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="25">
+        <f>F21*'Shotcrete Hang'!$B$13</f>
+        <v>4.1977361020938733E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>9.492483299759916E-3</v>
       </c>
@@ -4809,8 +4870,12 @@
         <f t="shared" si="2"/>
         <v>1.1106205460719101E-6</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="25">
+        <f>F22*'Shotcrete Hang'!$B$13</f>
+        <v>5.2664071425965485E-8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>9.492483299759916E-3</v>
       </c>
@@ -4835,8 +4900,12 @@
         <f t="shared" si="2"/>
         <v>6.3886311104044196E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="25">
+        <f>F23*'Shotcrete Hang'!$B$13</f>
+        <v>3.0293994317182304E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -4846,8 +4915,9 @@
       <c r="F24" s="25"/>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="25"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>5.0195800241836508E-2</v>
       </c>
@@ -4872,8 +4942,12 @@
         <f t="shared" si="2"/>
         <v>3.2476682756468219E-4</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="25">
+        <f>F25*'Shotcrete Hang'!$B$13</f>
+        <v>1.5399988289558642E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>5.0195800241836508E-2</v>
       </c>
@@ -4898,8 +4972,12 @@
         <f t="shared" si="2"/>
         <v>6.7764330326479288E-5</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="25">
+        <f>F26*'Shotcrete Hang'!$B$13</f>
+        <v>3.213289674019191E-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>5.0195800241836508E-2</v>
       </c>
@@ -4924,8 +5002,12 @@
         <f t="shared" si="2"/>
         <v>1.0470843930447094E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="25">
+        <f>F27*'Shotcrete Hang'!$B$13</f>
+        <v>4.9651276000029861E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>5.0195800241836508E-2</v>
       </c>
@@ -4950,8 +5032,12 @@
         <f t="shared" si="2"/>
         <v>2.0078320096734603E-6</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="25">
+        <f>F28*'Shotcrete Hang'!$B$13</f>
+        <v>9.5208582933901955E-8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>5.0195800241836508E-2</v>
       </c>
@@ -4976,8 +5062,12 @@
         <f t="shared" si="2"/>
         <v>9.3866146452234263E-5</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="25">
+        <f>F29*'Shotcrete Hang'!$B$13</f>
+        <v>4.4510012521599157E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>25</v>
       </c>
@@ -4987,8 +5077,9 @@
       <c r="F30" s="25"/>
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="25"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>1.4202133142682343E-3</v>
       </c>
@@ -5013,8 +5104,12 @@
         <f t="shared" si="2"/>
         <v>1.4202133142682343E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="25">
+        <f>F31*'Shotcrete Hang'!$B$13</f>
+        <v>6.7344527063959708E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>26</v>
       </c>
@@ -5024,8 +5119,9 @@
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="25"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>9.5912336284833428E-3</v>
       </c>
@@ -5050,8 +5146,12 @@
         <f t="shared" si="2"/>
         <v>5.6060760558485133E-4</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="25">
+        <f>F33*'Shotcrete Hang'!$B$13</f>
+        <v>2.6583227806185834E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>9.5912336284833428E-3</v>
       </c>
@@ -5076,8 +5176,12 @@
         <f t="shared" si="2"/>
         <v>8.8003405034786063E-3</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="25">
+        <f>F34*'Shotcrete Hang'!$B$13</f>
+        <v>4.172998261982507E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>9.5912336284833428E-3</v>
       </c>
@@ -5102,8 +5206,12 @@
         <f t="shared" si="2"/>
         <v>2.0323824058756206E-4</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="25">
+        <f>F35*'Shotcrete Hang'!$B$13</f>
+        <v>9.6372728351253717E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>9.5912336284833428E-3</v>
       </c>
@@ -5128,8 +5236,12 @@
         <f t="shared" si="2"/>
         <v>2.7047278832323025E-5</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I36" s="25">
+        <f>F36*'Shotcrete Hang'!$B$13</f>
+        <v>1.2825440960383927E-6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B37" s="16">
         <f>B2+B3+B5+B8+B10+B14+B16+B20+B24+B30+B32</f>
         <v>1</v>

</xml_diff>